<commit_message>
Disabled smart identification for the runs
</commit_message>
<xml_diff>
--- a/uft-one-traditional-or-ppm-ensure-logged-out/Default.xlsx
+++ b/uft-one-traditional-or-ppm-ensure-logged-out/Default.xlsx
@@ -181,7 +181,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -192,9 +194,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>1</v>
       </c>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>